<commit_message>
add chip and version info to init
</commit_message>
<xml_diff>
--- a/memory.xlsx
+++ b/memory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Different\Electronics\SportIDuino\siduino\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Different\Electronics\SportIDuino\sportiduino_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35A6606-954D-4BB0-9461-87FC83C00D19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF0CFA-2E48-4FA6-9FB8-04CE93DED4DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHIP" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="63">
   <si>
     <t>page</t>
   </si>
@@ -204,13 +204,16 @@
     <t>Мастер-чип очистки EEPROM</t>
   </si>
   <si>
-    <t>пароль 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">пароль 4 </t>
-  </si>
-  <si>
     <t>пароль NFC</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x69</t>
+  </si>
+  <si>
+    <t>пароль nfc</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -875,11 +878,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="27"/>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0</v>
+      <c r="D7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1476,7 +1479,7 @@
         <v>37</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,19 +2034,16 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B40:E43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B28:E31"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H28:K31"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H40:K43"/>
+    <mergeCell ref="H16:K19"/>
+    <mergeCell ref="B16:E19"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H4:K7"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A13:E13"/>
@@ -2054,16 +2054,19 @@
     <mergeCell ref="B4:E7"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E19"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H4:K7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H40:K43"/>
-    <mergeCell ref="H16:K19"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B28:E31"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H28:K31"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B40:E43"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -2074,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2502,7 @@
         <v>859</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -2514,7 +2517,7 @@
         <v>860</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -2529,7 +2532,7 @@
         <v>861</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -2761,6 +2764,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
     <mergeCell ref="B38:I38"/>
     <mergeCell ref="B34:I34"/>
     <mergeCell ref="B23:I23"/>
@@ -2777,22 +2796,6 @@
     <mergeCell ref="B31:I31"/>
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3930,11 +3933,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B14:AG19"/>
-    <mergeCell ref="J9:AG9"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B12:AG12"/>
-    <mergeCell ref="B1:AG1"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B5:AG8"/>
     <mergeCell ref="B3:I3"/>
@@ -3945,6 +3943,11 @@
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:Y2"/>
     <mergeCell ref="Z2:AG2"/>
+    <mergeCell ref="B14:AG19"/>
+    <mergeCell ref="J9:AG9"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B12:AG12"/>
+    <mergeCell ref="B1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>